<commit_message>
more type generation fixes and cleanup
</commit_message>
<xml_diff>
--- a/addons/binding/org.openhab.binding.smartthings/CapabilityMappings.xlsx
+++ b/addons/binding/org.openhab.binding.smartthings/CapabilityMappings.xlsx
@@ -3239,8 +3239,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A2:F260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A141" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26:F216"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A89" sqref="A89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3365,7 +3365,7 @@
         <v>attributeCommandMap.put("Alarm_alarm_strobe","strobe()");</v>
       </c>
     </row>
-    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -3373,7 +3373,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -3381,7 +3381,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -3389,7 +3389,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -3397,7 +3397,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -3405,7 +3405,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -3463,7 +3463,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>165</v>
       </c>
@@ -3563,7 +3563,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -3581,7 +3581,7 @@
         <v>attributeCommandMap.put("Color Control_color","setColor(COLOR_MAP)");</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -3599,7 +3599,7 @@
         <v>attributeCommandMap.put("Color Control_hue","setHue(NUMBER)");</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>21</v>
       </c>
@@ -3617,7 +3617,7 @@
         <v>attributeCommandMap.put("Color Control_saturation","setSaturation(NUMBER)");</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>25</v>
       </c>
@@ -3635,7 +3635,7 @@
         <v>attributeCommandMap.put("Color Temperature_colorTemperature","setColorTemperature(NUMBER)");</v>
       </c>
     </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>27</v>
       </c>
@@ -3839,7 +3839,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>32</v>
       </c>
@@ -3847,7 +3847,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>32</v>
       </c>
@@ -3947,7 +3947,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>39</v>
       </c>
@@ -3955,7 +3955,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>39</v>
       </c>
@@ -3974,7 +3974,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>166</v>
       </c>
@@ -4004,7 +4004,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>42</v>
       </c>
@@ -4184,7 +4184,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>50</v>
       </c>
@@ -4192,7 +4192,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>50</v>
       </c>
@@ -4278,7 +4278,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>163</v>
       </c>
@@ -4286,7 +4286,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>163</v>
       </c>
@@ -4294,7 +4294,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>163</v>
       </c>
@@ -4302,7 +4302,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>163</v>
       </c>
@@ -4310,7 +4310,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>163</v>
       </c>
@@ -4318,7 +4318,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>163</v>
       </c>
@@ -4326,7 +4326,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>163</v>
       </c>
@@ -4356,7 +4356,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>54</v>
       </c>
@@ -4364,7 +4364,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="87" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>54</v>
       </c>
@@ -4372,7 +4372,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="88" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>54</v>
       </c>
@@ -4380,7 +4380,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="89" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>59</v>
       </c>
@@ -4502,7 +4502,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="98" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>63</v>
       </c>
@@ -4510,7 +4510,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="99" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>63</v>
       </c>
@@ -4518,7 +4518,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="100" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>63</v>
       </c>
@@ -4526,7 +4526,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="101" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>63</v>
       </c>
@@ -4534,7 +4534,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="102" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>63</v>
       </c>
@@ -4542,7 +4542,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="103" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>63</v>
       </c>
@@ -4550,7 +4550,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="104" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>63</v>
       </c>
@@ -4558,7 +4558,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="105" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>63</v>
       </c>
@@ -4566,7 +4566,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="106" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>63</v>
       </c>
@@ -4574,7 +4574,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="107" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>63</v>
       </c>
@@ -4582,7 +4582,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="108" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>76</v>
       </c>
@@ -4601,7 +4601,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="110" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>79</v>
       </c>
@@ -4760,7 +4760,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>86</v>
       </c>
@@ -5119,7 +5119,7 @@
         <v>attributeCommandMap.put("Samsung TV_switch_on","on()");</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>168</v>
       </c>
@@ -5137,7 +5137,7 @@
         <v>attributeCommandMap.put("Samsung TV_volume","setVolume(NUMBER)");</v>
       </c>
     </row>
-    <row r="142" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>168</v>
       </c>
@@ -5145,7 +5145,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="143" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>168</v>
       </c>
@@ -5153,7 +5153,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="144" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>168</v>
       </c>
@@ -5331,7 +5331,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="158" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>107</v>
       </c>
@@ -5403,7 +5403,7 @@
         <v>attributeCommandMap.put("Switch_switch_on","on()");</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>112</v>
       </c>
@@ -5460,7 +5460,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>119</v>
       </c>
@@ -5478,7 +5478,7 @@
         <v>attributeCommandMap.put("Thermostat_coolingSetpoint","setCoolingSetpoint(NUMBER)");</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>119</v>
       </c>
@@ -5795,7 +5795,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="187" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>119</v>
       </c>
@@ -5803,7 +5803,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="188" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>119</v>
       </c>
@@ -5811,7 +5811,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="189" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>119</v>
       </c>
@@ -5819,7 +5819,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>133</v>
       </c>
@@ -5900,7 +5900,7 @@
         <v>attributeCommandMap.put("Thermostat Fan Mode_thermostatFanMode_on","fanOn()");</v>
       </c>
     </row>
-    <row r="194" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>134</v>
       </c>
@@ -5908,7 +5908,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>135</v>
       </c>
@@ -6031,7 +6031,7 @@
         <v>attributeCommandMap.put("Thermostat Mode_thermostatMode_off","off()");</v>
       </c>
     </row>
-    <row r="201" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>136</v>
       </c>
@@ -6137,7 +6137,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>161</v>
       </c>
@@ -6261,7 +6261,7 @@
         <v>attributeCommandMap.put("Timed Session_sessionStatus_stopped","stop()");</v>
       </c>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>141</v>
       </c>
@@ -6279,7 +6279,7 @@
         <v>attributeCommandMap.put("Timed Session_timeRemaining","setTimeRemaining(NUMBER)");</v>
       </c>
     </row>
-    <row r="217" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>146</v>
       </c>
@@ -6367,7 +6367,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="225" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>167</v>
       </c>
@@ -6375,7 +6375,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="226" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>167</v>
       </c>
@@ -6383,7 +6383,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="227" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>167</v>
       </c>
@@ -6391,7 +6391,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="228" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>167</v>
       </c>
@@ -6614,7 +6614,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="242" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>160</v>
       </c>
@@ -6633,7 +6633,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="244" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>169</v>
       </c>
@@ -6764,7 +6764,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="254" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>157</v>
       </c>
@@ -6794,7 +6794,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="257" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>170</v>
       </c>
@@ -6802,7 +6802,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="258" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>170</v>
       </c>
@@ -6810,7 +6810,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="259" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>157</v>
       </c>
@@ -6818,7 +6818,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="260" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>157</v>
       </c>
@@ -6829,11 +6829,7 @@
   </sheetData>
   <autoFilter ref="A1:H260">
     <filterColumn colId="2">
-      <filters>
-        <filter val="JSON_OBJECT"/>
-        <filter val="NUMBER"/>
-        <filter val="STRING"/>
-      </filters>
+      <filters blank="1"/>
     </filterColumn>
     <filterColumn colId="4">
       <customFilters>

</xml_diff>

<commit_message>
hard defining capabilities as channels
</commit_message>
<xml_diff>
--- a/addons/binding/org.openhab.binding.smartthings/CapabilityMappings.xlsx
+++ b/addons/binding/org.openhab.binding.smartthings/CapabilityMappings.xlsx
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">AttributeChannelMap!$A$1:$F$154</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">AttributeCommandMap!$A$1:$H$260</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">AttributeCommandMap!$A$1:$K$260</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1412" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1485" uniqueCount="312">
   <si>
     <t>Acceleration Sensor</t>
   </si>
@@ -954,6 +954,18 @@
   </si>
   <si>
     <t>epCmd(NUMBER,STRING)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>Dimmer</t>
+  </si>
+  <si>
+    <t>Number</t>
   </si>
 </sst>
 </file>
@@ -1682,10 +1694,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D154"/>
+  <dimension ref="A1:D154"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B154" sqref="B154"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1696,6 +1708,11 @@
     <col min="4" max="4" width="44" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>308</v>
+      </c>
+    </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
@@ -3237,10 +3254,11 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A2:F260"/>
+  <dimension ref="A2:I260"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A89" sqref="A89"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C201" sqref="C201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3250,10 +3268,12 @@
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="44" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="111.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="52.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="44" customWidth="1"/>
+    <col min="9" max="9" width="111.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3266,8 +3286,15 @@
       <c r="D2" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F2" t="str">
+        <f>CONCATENATE(SUBSTITUTE(A2," ","_"),"_",B2)</f>
+        <v>Acceleration_Sensor_acceleration</v>
+      </c>
+      <c r="G2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -3280,8 +3307,15 @@
       <c r="D3" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F3" t="str">
+        <f>CONCATENATE(SUBSTITUTE(A3," ","_"),"_",B3)</f>
+        <v>Acceleration_Sensor_acceleration</v>
+      </c>
+      <c r="G3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -3298,11 +3332,19 @@
         <v>8</v>
       </c>
       <c r="F4" t="str">
+        <f t="shared" ref="F4:F7" si="0">CONCATENATE(SUBSTITUTE(A4," ","_"),"_",B4)</f>
+        <v>Alarm_alarm</v>
+      </c>
+      <c r="H4" t="str">
+        <f>SUBSTITUTE(CONCATENATE(A4,"_",B4,IF(D4="","",CONCATENATE("_",D4)),":""",E4,""",")," ","_")</f>
+        <v>Alarm_alarm_both:"both()",</v>
+      </c>
+      <c r="I4" t="str">
         <f>CONCATENATE("attributeCommandMap.put(""",A4,"_",B4,"_",D4,""",""","",E4,""");")</f>
         <v>attributeCommandMap.put("Alarm_alarm_both","both()");</v>
       </c>
     </row>
-    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -3319,11 +3361,19 @@
         <v>5</v>
       </c>
       <c r="F5" t="str">
-        <f t="shared" ref="F5:F7" si="0">CONCATENATE("attributeCommandMap.put(""",A5,"_",B5,"_",D5,""",""","",E5,""");")</f>
+        <f t="shared" si="0"/>
+        <v>Alarm_alarm</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" ref="H5:H7" si="1">SUBSTITUTE(CONCATENATE(A5,"_",B5,IF(D5="","",CONCATENATE("_",D5)),":""",E5,""",")," ","_")</f>
+        <v>Alarm_alarm_off:"off()",</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" ref="I5:I7" si="2">CONCATENATE("attributeCommandMap.put(""",A5,"_",B5,"_",D5,""",""","",E5,""");")</f>
         <v>attributeCommandMap.put("Alarm_alarm_off","off()");</v>
       </c>
     </row>
-    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -3341,10 +3391,18 @@
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
+        <v>Alarm_alarm</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="1"/>
+        <v>Alarm_alarm_siren:"siren()",</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="2"/>
         <v>attributeCommandMap.put("Alarm_alarm_siren","siren()");</v>
       </c>
     </row>
-    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -3362,10 +3420,18 @@
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
+        <v>Alarm_alarm</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="1"/>
+        <v>Alarm_alarm_strobe:"strobe()",</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="2"/>
         <v>attributeCommandMap.put("Alarm_alarm_strobe","strobe()");</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -3373,7 +3439,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -3381,7 +3447,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -3389,7 +3455,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -3397,7 +3463,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -3405,7 +3471,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -3413,7 +3479,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -3423,8 +3489,15 @@
       <c r="C14" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F14" t="str">
+        <f>CONCATENATE(SUBSTITUTE(A14," ","_"),"_",B14)</f>
+        <v>Battery_battery</v>
+      </c>
+      <c r="G14" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -3437,8 +3510,15 @@
       <c r="D15" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F15" t="str">
+        <f t="shared" ref="F15:F35" si="3">CONCATENATE(SUBSTITUTE(A15," ","_"),"_",B15)</f>
+        <v>Beacon_presence</v>
+      </c>
+      <c r="G15" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -3451,8 +3531,15 @@
       <c r="D16" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F16" t="str">
+        <f>CONCATENATE(SUBSTITUTE(A16," ","_"),"_",B16)</f>
+        <v>Beacon_presence</v>
+      </c>
+      <c r="G16" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>165</v>
       </c>
@@ -3462,8 +3549,12 @@
       <c r="C17" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F17" t="str">
+        <f t="shared" si="3"/>
+        <v>Buffered_Video_Capture_clip</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>165</v>
       </c>
@@ -3471,7 +3562,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -3484,8 +3575,12 @@
       <c r="D19" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F19" t="str">
+        <f t="shared" si="3"/>
+        <v>Button_button</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -3498,8 +3593,12 @@
       <c r="D20" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F20" t="str">
+        <f t="shared" si="3"/>
+        <v>Button_button</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -3509,8 +3608,15 @@
       <c r="C21" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F21" t="str">
+        <f t="shared" si="3"/>
+        <v>Button_numberOfButtons</v>
+      </c>
+      <c r="G21" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -3520,8 +3626,15 @@
       <c r="C22" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F22" t="str">
+        <f t="shared" si="3"/>
+        <v>Carbon_Dioxide_Measurement_carbonDioxide</v>
+      </c>
+      <c r="G22" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -3534,8 +3647,12 @@
       <c r="D23" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F23" t="str">
+        <f t="shared" si="3"/>
+        <v>Carbon_Monoxide_Detector_carbonMonoxide</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -3548,8 +3665,12 @@
       <c r="D24" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F24" t="str">
+        <f t="shared" si="3"/>
+        <v>Carbon_Monoxide_Detector_carbonMonoxide</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>19</v>
       </c>
@@ -3562,8 +3683,12 @@
       <c r="D25" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F25" t="str">
+        <f t="shared" si="3"/>
+        <v>Carbon_Monoxide_Detector_carbonMonoxide</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -3577,11 +3702,19 @@
         <v>278</v>
       </c>
       <c r="F26" t="str">
+        <f t="shared" si="3"/>
+        <v>Color_Control_color</v>
+      </c>
+      <c r="H26" t="str">
+        <f t="shared" ref="H26:H29" si="4">SUBSTITUTE(CONCATENATE(A26,"_",B26,IF(D26="","",CONCATENATE("_",D26)),":""",E26,""",")," ","_")</f>
+        <v>Color_Control_color:"setColor(COLOR_MAP)",</v>
+      </c>
+      <c r="I26" t="str">
         <f>CONCATENATE("attributeCommandMap.put(""",A26,"_",B26,""",""","",E26,""");")</f>
         <v>attributeCommandMap.put("Color Control_color","setColor(COLOR_MAP)");</v>
       </c>
     </row>
-    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -3595,11 +3728,22 @@
         <v>279</v>
       </c>
       <c r="F27" t="str">
-        <f t="shared" ref="F27:F29" si="1">CONCATENATE("attributeCommandMap.put(""",A27,"_",B27,""",""","",E27,""");")</f>
+        <f t="shared" si="3"/>
+        <v>Color_Control_hue</v>
+      </c>
+      <c r="G27" t="s">
+        <v>311</v>
+      </c>
+      <c r="H27" t="str">
+        <f t="shared" si="4"/>
+        <v>Color_Control_hue:"setHue(NUMBER)",</v>
+      </c>
+      <c r="I27" t="str">
+        <f t="shared" ref="I27:I29" si="5">CONCATENATE("attributeCommandMap.put(""",A27,"_",B27,""",""","",E27,""");")</f>
         <v>attributeCommandMap.put("Color Control_hue","setHue(NUMBER)");</v>
       </c>
     </row>
-    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>21</v>
       </c>
@@ -3613,11 +3757,22 @@
         <v>280</v>
       </c>
       <c r="F28" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
+        <v>Color_Control_saturation</v>
+      </c>
+      <c r="G28" t="s">
+        <v>311</v>
+      </c>
+      <c r="H28" t="str">
+        <f t="shared" si="4"/>
+        <v>Color_Control_saturation:"setSaturation(NUMBER)",</v>
+      </c>
+      <c r="I28" t="str">
+        <f t="shared" si="5"/>
         <v>attributeCommandMap.put("Color Control_saturation","setSaturation(NUMBER)");</v>
       </c>
     </row>
-    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>25</v>
       </c>
@@ -3631,11 +3786,22 @@
         <v>281</v>
       </c>
       <c r="F29" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
+        <v>Color_Temperature_colorTemperature</v>
+      </c>
+      <c r="G29" t="s">
+        <v>311</v>
+      </c>
+      <c r="H29" t="str">
+        <f t="shared" si="4"/>
+        <v>Color_Temperature_colorTemperature:"setColorTemperature(NUMBER)",</v>
+      </c>
+      <c r="I29" t="str">
+        <f t="shared" si="5"/>
         <v>attributeCommandMap.put("Color Temperature_colorTemperature","setColorTemperature(NUMBER)");</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>27</v>
       </c>
@@ -3643,7 +3809,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -3656,8 +3822,12 @@
       <c r="D31" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F31" t="str">
+        <f t="shared" si="3"/>
+        <v>Consumable_consumableStatus</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -3674,11 +3844,19 @@
         <v>282</v>
       </c>
       <c r="F32" t="str">
-        <f t="shared" ref="F32:F35" si="2">CONCATENATE("attributeCommandMap.put(""",A32,"_",B32,"_",D32,""",""","",E32,""");")</f>
+        <f t="shared" si="3"/>
+        <v>Consumable_consumableStatus</v>
+      </c>
+      <c r="H32" t="str">
+        <f t="shared" ref="H32:H35" si="6">SUBSTITUTE(CONCATENATE(A32,"_",B32,IF(D32="","",CONCATENATE("_",D32)),":""",E32,""",")," ","_")</f>
+        <v>Consumable_consumableStatus_maintenance_required:"setConsumableStatus(STRING)",</v>
+      </c>
+      <c r="I32" t="str">
+        <f t="shared" ref="I32:I35" si="7">CONCATENATE("attributeCommandMap.put(""",A32,"_",B32,"_",D32,""",""","",E32,""");")</f>
         <v>attributeCommandMap.put("Consumable_consumableStatus_maintenance_required","setConsumableStatus(STRING)");</v>
       </c>
     </row>
-    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>29</v>
       </c>
@@ -3695,11 +3873,19 @@
         <v>282</v>
       </c>
       <c r="F33" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>Consumable_consumableStatus</v>
+      </c>
+      <c r="H33" t="str">
+        <f t="shared" si="6"/>
+        <v>Consumable_consumableStatus_missing:"setConsumableStatus(STRING)",</v>
+      </c>
+      <c r="I33" t="str">
+        <f t="shared" si="7"/>
         <v>attributeCommandMap.put("Consumable_consumableStatus_missing","setConsumableStatus(STRING)");</v>
       </c>
     </row>
-    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>29</v>
       </c>
@@ -3716,11 +3902,19 @@
         <v>282</v>
       </c>
       <c r="F34" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>Consumable_consumableStatus</v>
+      </c>
+      <c r="H34" t="str">
+        <f t="shared" si="6"/>
+        <v>Consumable_consumableStatus_order:"setConsumableStatus(STRING)",</v>
+      </c>
+      <c r="I34" t="str">
+        <f t="shared" si="7"/>
         <v>attributeCommandMap.put("Consumable_consumableStatus_order","setConsumableStatus(STRING)");</v>
       </c>
     </row>
-    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>29</v>
       </c>
@@ -3737,11 +3931,19 @@
         <v>282</v>
       </c>
       <c r="F35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>Consumable_consumableStatus</v>
+      </c>
+      <c r="H35" t="str">
+        <f t="shared" si="6"/>
+        <v>Consumable_consumableStatus_replace:"setConsumableStatus(STRING)",</v>
+      </c>
+      <c r="I35" t="str">
+        <f t="shared" si="7"/>
         <v>attributeCommandMap.put("Consumable_consumableStatus_replace","setConsumableStatus(STRING)");</v>
       </c>
     </row>
-    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>30</v>
       </c>
@@ -3754,8 +3956,15 @@
       <c r="D36" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F36" t="str">
+        <f t="shared" ref="F36:F42" si="8">CONCATENATE(SUBSTITUTE(A36," ","_"),"_",B36)</f>
+        <v>Contact_Sensor_contact</v>
+      </c>
+      <c r="G36" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>30</v>
       </c>
@@ -3768,8 +3977,15 @@
       <c r="D37" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F37" t="str">
+        <f t="shared" si="8"/>
+        <v>Contact_Sensor_contact</v>
+      </c>
+      <c r="G37" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>32</v>
       </c>
@@ -3782,8 +3998,12 @@
       <c r="D38" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F38" t="str">
+        <f t="shared" si="8"/>
+        <v>Door_Control_door</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>32</v>
       </c>
@@ -3796,8 +4016,12 @@
       <c r="D39" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F39" t="str">
+        <f t="shared" si="8"/>
+        <v>Door_Control_door</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>32</v>
       </c>
@@ -3810,8 +4034,12 @@
       <c r="D40" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F40" t="str">
+        <f t="shared" si="8"/>
+        <v>Door_Control_door</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>32</v>
       </c>
@@ -3824,8 +4052,12 @@
       <c r="D41" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F41" t="str">
+        <f t="shared" si="8"/>
+        <v>Door_Control_door</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>32</v>
       </c>
@@ -3838,8 +4070,12 @@
       <c r="D42" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F42" t="str">
+        <f t="shared" si="8"/>
+        <v>Door_Control_door</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>32</v>
       </c>
@@ -3847,7 +4083,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>32</v>
       </c>
@@ -3855,7 +4091,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>36</v>
       </c>
@@ -3865,8 +4101,15 @@
       <c r="C45" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F45" t="str">
+        <f t="shared" ref="F45:F51" si="9">CONCATENATE(SUBSTITUTE(A45," ","_"),"_",B45)</f>
+        <v>Energy_Meter_energy</v>
+      </c>
+      <c r="G45" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>172</v>
       </c>
@@ -3876,8 +4119,12 @@
       <c r="C46" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F46" t="str">
+        <f t="shared" si="9"/>
+        <v>Estimated_Time_Of_Arrival_eta</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>39</v>
       </c>
@@ -3890,8 +4137,12 @@
       <c r="D47" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F47" t="str">
+        <f t="shared" si="9"/>
+        <v>Garage_Door_Control_door</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>39</v>
       </c>
@@ -3904,8 +4155,12 @@
       <c r="D48" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F48" t="str">
+        <f t="shared" si="9"/>
+        <v>Garage_Door_Control_door</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>39</v>
       </c>
@@ -3918,8 +4173,12 @@
       <c r="D49" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F49" t="str">
+        <f t="shared" si="9"/>
+        <v>Garage_Door_Control_door</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>39</v>
       </c>
@@ -3932,8 +4191,12 @@
       <c r="D50" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F50" t="str">
+        <f t="shared" si="9"/>
+        <v>Garage_Door_Control_door</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>39</v>
       </c>
@@ -3946,8 +4209,12 @@
       <c r="D51" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F51" t="str">
+        <f t="shared" si="9"/>
+        <v>Garage_Door_Control_door</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>39</v>
       </c>
@@ -3955,7 +4222,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>39</v>
       </c>
@@ -3963,7 +4230,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>166</v>
       </c>
@@ -3973,8 +4240,15 @@
       <c r="C54" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F54" t="str">
+        <f t="shared" ref="F54" si="10">CONCATENATE(SUBSTITUTE(A54," ","_"),"_",B54)</f>
+        <v>Health_Check_checkInterval</v>
+      </c>
+      <c r="G54" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>166</v>
       </c>
@@ -3982,7 +4256,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>40</v>
       </c>
@@ -3992,8 +4266,15 @@
       <c r="C56" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F56" t="str">
+        <f t="shared" ref="F56:F57" si="11">CONCATENATE(SUBSTITUTE(A56," ","_"),"_",B56)</f>
+        <v>Illuminance_Measurement_illuminance</v>
+      </c>
+      <c r="G56" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>42</v>
       </c>
@@ -4003,8 +4284,12 @@
       <c r="C57" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F57" t="str">
+        <f t="shared" si="11"/>
+        <v>Image_Capture_image</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>42</v>
       </c>
@@ -4012,7 +4297,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>45</v>
       </c>
@@ -4029,11 +4314,19 @@
         <v>49</v>
       </c>
       <c r="F59" t="str">
-        <f t="shared" ref="F59:F63" si="3">CONCATENATE("attributeCommandMap.put(""",A59,"_",B59,"_",D59,""",""","",E59,""");")</f>
+        <f t="shared" ref="F59:F61" si="12">CONCATENATE(SUBSTITUTE(A59," ","_"),"_",B59)</f>
+        <v>Indicator_indicatorStatus</v>
+      </c>
+      <c r="H59" t="str">
+        <f t="shared" ref="H59:H63" si="13">SUBSTITUTE(CONCATENATE(A59,"_",B59,IF(D59="","",CONCATENATE("_",D59)),":""",E59,""",")," ","_")</f>
+        <v>Indicator_indicatorStatus_never:"indicatorNever()",</v>
+      </c>
+      <c r="I59" t="str">
+        <f t="shared" ref="I59:I63" si="14">CONCATENATE("attributeCommandMap.put(""",A59,"_",B59,"_",D59,""",""","",E59,""");")</f>
         <v>attributeCommandMap.put("Indicator_indicatorStatus_never","indicatorNever()");</v>
       </c>
     </row>
-    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>45</v>
       </c>
@@ -4050,11 +4343,19 @@
         <v>48</v>
       </c>
       <c r="F60" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
+        <v>Indicator_indicatorStatus</v>
+      </c>
+      <c r="H60" t="str">
+        <f t="shared" si="13"/>
+        <v>Indicator_indicatorStatus_when_off:"indicatorWhenOff()",</v>
+      </c>
+      <c r="I60" t="str">
+        <f t="shared" si="14"/>
         <v>attributeCommandMap.put("Indicator_indicatorStatus_when off","indicatorWhenOff()");</v>
       </c>
     </row>
-    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>45</v>
       </c>
@@ -4071,11 +4372,19 @@
         <v>47</v>
       </c>
       <c r="F61" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
+        <v>Indicator_indicatorStatus</v>
+      </c>
+      <c r="H61" t="str">
+        <f t="shared" si="13"/>
+        <v>Indicator_indicatorStatus_when_on:"indicatorWhenOn()",</v>
+      </c>
+      <c r="I61" t="str">
+        <f t="shared" si="14"/>
         <v>attributeCommandMap.put("Indicator_indicatorStatus_when on","indicatorWhenOn()");</v>
       </c>
     </row>
-    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>164</v>
       </c>
@@ -4092,11 +4401,22 @@
         <v>5</v>
       </c>
       <c r="F62" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="F62:F68" si="15">CONCATENATE(SUBSTITUTE(A62," ","_"),"_",B62)</f>
+        <v>Light_switch</v>
+      </c>
+      <c r="G62" t="s">
+        <v>111</v>
+      </c>
+      <c r="H62" t="str">
+        <f t="shared" si="13"/>
+        <v>Light_switch_off:"off()",</v>
+      </c>
+      <c r="I62" t="str">
+        <f t="shared" si="14"/>
         <v>attributeCommandMap.put("Light_switch_off","off()");</v>
       </c>
     </row>
-    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>164</v>
       </c>
@@ -4113,11 +4433,22 @@
         <v>92</v>
       </c>
       <c r="F63" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
+        <v>Light_switch</v>
+      </c>
+      <c r="G63" t="s">
+        <v>111</v>
+      </c>
+      <c r="H63" t="str">
+        <f t="shared" si="13"/>
+        <v>Light_switch_on:"on()",</v>
+      </c>
+      <c r="I63" t="str">
+        <f t="shared" si="14"/>
         <v>attributeCommandMap.put("Light_switch_on","on()");</v>
       </c>
     </row>
-    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>173</v>
       </c>
@@ -4127,8 +4458,12 @@
       <c r="C64" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F64" t="str">
+        <f t="shared" si="15"/>
+        <v>Location_Mode_mode</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>50</v>
       </c>
@@ -4141,8 +4476,12 @@
       <c r="D65" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F65" t="str">
+        <f t="shared" si="15"/>
+        <v>Lock_lock</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>50</v>
       </c>
@@ -4155,8 +4494,12 @@
       <c r="D66" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F66" t="str">
+        <f t="shared" si="15"/>
+        <v>Lock_lock</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>50</v>
       </c>
@@ -4169,8 +4512,12 @@
       <c r="D67" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F67" t="str">
+        <f t="shared" si="15"/>
+        <v>Lock_lock</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>50</v>
       </c>
@@ -4183,8 +4530,12 @@
       <c r="D68" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F68" t="str">
+        <f t="shared" si="15"/>
+        <v>Lock_lock</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>50</v>
       </c>
@@ -4192,7 +4543,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>50</v>
       </c>
@@ -4200,7 +4551,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>163</v>
       </c>
@@ -4210,8 +4561,12 @@
       <c r="C71" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F71" t="str">
+        <f t="shared" ref="F71:F76" si="16">CONCATENATE(SUBSTITUTE(A71," ","_"),"_",B71)</f>
+        <v>Lock_Codes_codeChanged</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>163</v>
       </c>
@@ -4221,8 +4576,12 @@
       <c r="C72" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F72" t="str">
+        <f t="shared" si="16"/>
+        <v>Lock_Codes_codeReport</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>163</v>
       </c>
@@ -4235,8 +4594,12 @@
       <c r="D73" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F73" t="str">
+        <f t="shared" si="16"/>
+        <v>Lock_Codes_lock</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>163</v>
       </c>
@@ -4249,8 +4612,12 @@
       <c r="D74" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F74" t="str">
+        <f t="shared" si="16"/>
+        <v>Lock_Codes_lock</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>163</v>
       </c>
@@ -4263,8 +4630,12 @@
       <c r="D75" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F75" t="str">
+        <f t="shared" si="16"/>
+        <v>Lock_Codes_lock</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>163</v>
       </c>
@@ -4277,8 +4648,12 @@
       <c r="D76" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F76" t="str">
+        <f t="shared" si="16"/>
+        <v>Lock_Codes_lock</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>163</v>
       </c>
@@ -4286,7 +4661,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>163</v>
       </c>
@@ -4294,7 +4669,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>163</v>
       </c>
@@ -4302,7 +4677,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>163</v>
       </c>
@@ -4310,7 +4685,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>163</v>
       </c>
@@ -4318,7 +4693,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>163</v>
       </c>
@@ -4326,7 +4701,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>163</v>
       </c>
@@ -4334,7 +4709,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>54</v>
       </c>
@@ -4344,8 +4719,12 @@
       <c r="C84" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F84" t="str">
+        <f t="shared" ref="F84:F85" si="17">CONCATENATE(SUBSTITUTE(A84," ","_"),"_",B84)</f>
+        <v>Media_Controller_activities</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>54</v>
       </c>
@@ -4355,8 +4734,12 @@
       <c r="C85" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F85" t="str">
+        <f t="shared" si="17"/>
+        <v>Media_Controller_currentActivity</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>54</v>
       </c>
@@ -4364,7 +4747,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>54</v>
       </c>
@@ -4372,7 +4755,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>54</v>
       </c>
@@ -4380,7 +4763,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>59</v>
       </c>
@@ -4388,7 +4771,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="90" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>61</v>
       </c>
@@ -4401,8 +4784,15 @@
       <c r="D90" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F90" t="str">
+        <f t="shared" ref="F90:F92" si="18">CONCATENATE(SUBSTITUTE(A90," ","_"),"_",B90)</f>
+        <v>Motion_Sensor_motion</v>
+      </c>
+      <c r="G90" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>61</v>
       </c>
@@ -4415,8 +4805,15 @@
       <c r="D91" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F91" t="str">
+        <f t="shared" si="18"/>
+        <v>Motion_Sensor_motion</v>
+      </c>
+      <c r="G91" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>63</v>
       </c>
@@ -4426,8 +4823,15 @@
       <c r="C92" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F92" t="str">
+        <f t="shared" si="18"/>
+        <v>Music_Player_level</v>
+      </c>
+      <c r="G92" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>63</v>
       </c>
@@ -4444,11 +4848,22 @@
         <v>73</v>
       </c>
       <c r="F93" t="str">
-        <f t="shared" ref="F93:F94" si="4">CONCATENATE("attributeCommandMap.put(""",A93,"_",B93,"_",D93,""",""","",E93,""");")</f>
+        <f t="shared" ref="F93:F97" si="19">CONCATENATE(SUBSTITUTE(A93," ","_"),"_",B93)</f>
+        <v>Music_Player_mute</v>
+      </c>
+      <c r="G93" t="s">
+        <v>111</v>
+      </c>
+      <c r="H93" t="str">
+        <f t="shared" ref="H93:H94" si="20">SUBSTITUTE(CONCATENATE(A93,"_",B93,IF(D93="","",CONCATENATE("_",D93)),":""",E93,""",")," ","_")</f>
+        <v>Music_Player_mute_muted:"mute()",</v>
+      </c>
+      <c r="I93" t="str">
+        <f t="shared" ref="I93:I94" si="21">CONCATENATE("attributeCommandMap.put(""",A93,"_",B93,"_",D93,""",""","",E93,""");")</f>
         <v>attributeCommandMap.put("Music Player_mute_muted","mute()");</v>
       </c>
     </row>
-    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>63</v>
       </c>
@@ -4465,11 +4880,22 @@
         <v>75</v>
       </c>
       <c r="F94" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="19"/>
+        <v>Music_Player_mute</v>
+      </c>
+      <c r="G94" t="s">
+        <v>111</v>
+      </c>
+      <c r="H94" t="str">
+        <f t="shared" si="20"/>
+        <v>Music_Player_mute_unmuted:"unmute()",</v>
+      </c>
+      <c r="I94" t="str">
+        <f t="shared" si="21"/>
         <v>attributeCommandMap.put("Music Player_mute_unmuted","unmute()");</v>
       </c>
     </row>
-    <row r="95" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>63</v>
       </c>
@@ -4479,8 +4905,12 @@
       <c r="C95" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F95" t="str">
+        <f t="shared" si="19"/>
+        <v>Music_Player_status</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>63</v>
       </c>
@@ -4490,8 +4920,12 @@
       <c r="C96" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F96" t="str">
+        <f t="shared" si="19"/>
+        <v>Music_Player_trackData</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>63</v>
       </c>
@@ -4501,8 +4935,12 @@
       <c r="C97" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F97" t="str">
+        <f t="shared" si="19"/>
+        <v>Music_Player_trackDescription</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>63</v>
       </c>
@@ -4510,7 +4948,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>63</v>
       </c>
@@ -4518,7 +4956,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>63</v>
       </c>
@@ -4526,7 +4964,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>63</v>
       </c>
@@ -4534,7 +4972,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>63</v>
       </c>
@@ -4542,7 +4980,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>63</v>
       </c>
@@ -4550,7 +4988,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>63</v>
       </c>
@@ -4558,7 +4996,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>63</v>
       </c>
@@ -4566,7 +5004,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>63</v>
       </c>
@@ -4574,7 +5012,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>63</v>
       </c>
@@ -4582,7 +5020,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>76</v>
       </c>
@@ -4590,7 +5028,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="109" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>77</v>
       </c>
@@ -4600,8 +5038,15 @@
       <c r="C109" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F109" t="str">
+        <f t="shared" ref="F109" si="22">CONCATENATE(SUBSTITUTE(A109," ","_"),"_",B109)</f>
+        <v>pH_Measurement_pH</v>
+      </c>
+      <c r="G109" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>79</v>
       </c>
@@ -4609,7 +5054,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="111" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>83</v>
       </c>
@@ -4622,8 +5067,12 @@
       <c r="D111" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F111" t="str">
+        <f t="shared" ref="F111:F119" si="23">CONCATENATE(SUBSTITUTE(A111," ","_"),"_",B111)</f>
+        <v>Power_powerSource</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>83</v>
       </c>
@@ -4636,8 +5085,12 @@
       <c r="D112" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="113" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F112" t="str">
+        <f t="shared" si="23"/>
+        <v>Power_powerSource</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>83</v>
       </c>
@@ -4650,8 +5103,12 @@
       <c r="D113" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F113" t="str">
+        <f t="shared" si="23"/>
+        <v>Power_powerSource</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>83</v>
       </c>
@@ -4664,8 +5121,12 @@
       <c r="D114" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F114" t="str">
+        <f t="shared" si="23"/>
+        <v>Power_powerSource</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>81</v>
       </c>
@@ -4675,8 +5136,15 @@
       <c r="C115" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F115" t="str">
+        <f t="shared" si="23"/>
+        <v>Power_Meter_power</v>
+      </c>
+      <c r="G115" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>162</v>
       </c>
@@ -4689,8 +5157,12 @@
       <c r="D116" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F116" t="str">
+        <f t="shared" si="23"/>
+        <v>Power_Source_powerSource</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>162</v>
       </c>
@@ -4703,8 +5175,12 @@
       <c r="D117" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F117" t="str">
+        <f t="shared" si="23"/>
+        <v>Power_Source_powerSource</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>162</v>
       </c>
@@ -4717,8 +5193,12 @@
       <c r="D118" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F118" t="str">
+        <f t="shared" si="23"/>
+        <v>Power_Source_powerSource</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>162</v>
       </c>
@@ -4731,8 +5211,12 @@
       <c r="D119" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F119" t="str">
+        <f t="shared" si="23"/>
+        <v>Power_Source_powerSource</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>85</v>
       </c>
@@ -4745,8 +5229,15 @@
       <c r="D120" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F120" t="str">
+        <f t="shared" ref="F120:F123" si="24">CONCATENATE(SUBSTITUTE(A120," ","_"),"_",B120)</f>
+        <v>Presence_Sensor_presence</v>
+      </c>
+      <c r="G120" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>85</v>
       </c>
@@ -4759,8 +5250,15 @@
       <c r="D121" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F121" t="str">
+        <f t="shared" si="24"/>
+        <v>Presence_Sensor_presence</v>
+      </c>
+      <c r="G121" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>86</v>
       </c>
@@ -4768,7 +5266,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>88</v>
       </c>
@@ -4778,8 +5276,15 @@
       <c r="C123" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F123" t="str">
+        <f t="shared" si="24"/>
+        <v>Relative_Humidity_Measurement_humidity</v>
+      </c>
+      <c r="G123" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>90</v>
       </c>
@@ -4796,11 +5301,22 @@
         <v>5</v>
       </c>
       <c r="F124" t="str">
-        <f t="shared" ref="F124:F125" si="5">CONCATENATE("attributeCommandMap.put(""",A124,"_",B124,"_",D124,""",""","",E124,""");")</f>
+        <f t="shared" ref="F124:F126" si="25">CONCATENATE(SUBSTITUTE(A124," ","_"),"_",B124)</f>
+        <v>Relay_Switch_switch</v>
+      </c>
+      <c r="G124" t="s">
+        <v>111</v>
+      </c>
+      <c r="H124" t="str">
+        <f t="shared" ref="H124:H125" si="26">SUBSTITUTE(CONCATENATE(A124,"_",B124,IF(D124="","",CONCATENATE("_",D124)),":""",E124,""",")," ","_")</f>
+        <v>Relay_Switch_switch_off:"off()",</v>
+      </c>
+      <c r="I124" t="str">
+        <f t="shared" ref="I124:I125" si="27">CONCATENATE("attributeCommandMap.put(""",A124,"_",B124,"_",D124,""",""","",E124,""");")</f>
         <v>attributeCommandMap.put("Relay Switch_switch_off","off()");</v>
       </c>
     </row>
-    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>90</v>
       </c>
@@ -4817,11 +5333,22 @@
         <v>92</v>
       </c>
       <c r="F125" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="25"/>
+        <v>Relay_Switch_switch</v>
+      </c>
+      <c r="G125" t="s">
+        <v>111</v>
+      </c>
+      <c r="H125" t="str">
+        <f t="shared" si="26"/>
+        <v>Relay_Switch_switch_on:"on()",</v>
+      </c>
+      <c r="I125" t="str">
+        <f t="shared" si="27"/>
         <v>attributeCommandMap.put("Relay Switch_switch_on","on()");</v>
       </c>
     </row>
-    <row r="126" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>168</v>
       </c>
@@ -4831,8 +5358,12 @@
       <c r="C126" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="127" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F126" t="str">
+        <f t="shared" si="25"/>
+        <v>Samsung_TV_messageButton</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>168</v>
       </c>
@@ -4849,11 +5380,22 @@
         <v>73</v>
       </c>
       <c r="F127" t="str">
+        <f t="shared" ref="F127:F138" si="28">CONCATENATE(SUBSTITUTE(A127," ","_"),"_",B127)</f>
+        <v>Samsung_TV_mute</v>
+      </c>
+      <c r="G127" t="s">
+        <v>111</v>
+      </c>
+      <c r="H127" t="str">
+        <f>SUBSTITUTE(CONCATENATE(A127,"_",B127,IF(D127="","",CONCATENATE("_",D127)),":""",E127,""",")," ","_")</f>
+        <v>Samsung_TV_mute_muted:"mute()",</v>
+      </c>
+      <c r="I127" t="str">
         <f>CONCATENATE("attributeCommandMap.put(""",A127,"_",B127,"_",D127,""",""","",E127,""");")</f>
         <v>attributeCommandMap.put("Samsung TV_mute_muted","mute()");</v>
       </c>
     </row>
-    <row r="128" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>168</v>
       </c>
@@ -4866,8 +5408,15 @@
       <c r="D128" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="129" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F128" t="str">
+        <f t="shared" si="28"/>
+        <v>Samsung_TV_mute</v>
+      </c>
+      <c r="G128" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>168</v>
       </c>
@@ -4884,11 +5433,22 @@
         <v>75</v>
       </c>
       <c r="F129" t="str">
-        <f t="shared" ref="F129:F140" si="6">CONCATENATE("attributeCommandMap.put(""",A129,"_",B129,"_",D129,""",""","",E129,""");")</f>
+        <f t="shared" si="28"/>
+        <v>Samsung_TV_mute</v>
+      </c>
+      <c r="G129" t="s">
+        <v>111</v>
+      </c>
+      <c r="H129" t="str">
+        <f t="shared" ref="H129:H141" si="29">SUBSTITUTE(CONCATENATE(A129,"_",B129,IF(D129="","",CONCATENATE("_",D129)),":""",E129,""",")," ","_")</f>
+        <v>Samsung_TV_mute_unmuted:"unmute()",</v>
+      </c>
+      <c r="I129" t="str">
+        <f t="shared" ref="I129:I140" si="30">CONCATENATE("attributeCommandMap.put(""",A129,"_",B129,"_",D129,""",""","",E129,""");")</f>
         <v>attributeCommandMap.put("Samsung TV_mute_unmuted","unmute()");</v>
       </c>
     </row>
-    <row r="130" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>168</v>
       </c>
@@ -4905,11 +5465,19 @@
         <v>294</v>
       </c>
       <c r="F130" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="28"/>
+        <v>Samsung_TV_pictureMode</v>
+      </c>
+      <c r="H130" t="str">
+        <f t="shared" si="29"/>
+        <v>Samsung_TV_pictureMode_dynamic:"setPictureMode(ENUM)",</v>
+      </c>
+      <c r="I130" t="str">
+        <f t="shared" si="30"/>
         <v>attributeCommandMap.put("Samsung TV_pictureMode_dynamic","setPictureMode(ENUM)");</v>
       </c>
     </row>
-    <row r="131" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>168</v>
       </c>
@@ -4926,11 +5494,19 @@
         <v>294</v>
       </c>
       <c r="F131" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="28"/>
+        <v>Samsung_TV_pictureMode</v>
+      </c>
+      <c r="H131" t="str">
+        <f t="shared" si="29"/>
+        <v>Samsung_TV_pictureMode_movie:"setPictureMode(ENUM)",</v>
+      </c>
+      <c r="I131" t="str">
+        <f t="shared" si="30"/>
         <v>attributeCommandMap.put("Samsung TV_pictureMode_movie","setPictureMode(ENUM)");</v>
       </c>
     </row>
-    <row r="132" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>168</v>
       </c>
@@ -4947,11 +5523,19 @@
         <v>294</v>
       </c>
       <c r="F132" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="28"/>
+        <v>Samsung_TV_pictureMode</v>
+      </c>
+      <c r="H132" t="str">
+        <f t="shared" si="29"/>
+        <v>Samsung_TV_pictureMode_standard:"setPictureMode(ENUM)",</v>
+      </c>
+      <c r="I132" t="str">
+        <f t="shared" si="30"/>
         <v>attributeCommandMap.put("Samsung TV_pictureMode_standard","setPictureMode(ENUM)");</v>
       </c>
     </row>
-    <row r="133" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>168</v>
       </c>
@@ -4968,11 +5552,19 @@
         <v>294</v>
       </c>
       <c r="F133" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="28"/>
+        <v>Samsung_TV_pictureMode</v>
+      </c>
+      <c r="H133" t="str">
+        <f t="shared" si="29"/>
+        <v>Samsung_TV_pictureMode_unknown:"setPictureMode(ENUM)",</v>
+      </c>
+      <c r="I133" t="str">
+        <f t="shared" si="30"/>
         <v>attributeCommandMap.put("Samsung TV_pictureMode_unknown","setPictureMode(ENUM)");</v>
       </c>
     </row>
-    <row r="134" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>168</v>
       </c>
@@ -4989,11 +5581,19 @@
         <v>295</v>
       </c>
       <c r="F134" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="28"/>
+        <v>Samsung_TV_soundMode</v>
+      </c>
+      <c r="H134" t="str">
+        <f t="shared" si="29"/>
+        <v>Samsung_TV_soundMode_clear_voice:"setSoundMode(ENUM)",</v>
+      </c>
+      <c r="I134" t="str">
+        <f t="shared" si="30"/>
         <v>attributeCommandMap.put("Samsung TV_soundMode_clear voice","setSoundMode(ENUM)");</v>
       </c>
     </row>
-    <row r="135" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>168</v>
       </c>
@@ -5010,11 +5610,19 @@
         <v>295</v>
       </c>
       <c r="F135" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="28"/>
+        <v>Samsung_TV_soundMode</v>
+      </c>
+      <c r="H135" t="str">
+        <f t="shared" si="29"/>
+        <v>Samsung_TV_soundMode_movie:"setSoundMode(ENUM)",</v>
+      </c>
+      <c r="I135" t="str">
+        <f t="shared" si="30"/>
         <v>attributeCommandMap.put("Samsung TV_soundMode_movie","setSoundMode(ENUM)");</v>
       </c>
     </row>
-    <row r="136" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>168</v>
       </c>
@@ -5031,11 +5639,19 @@
         <v>295</v>
       </c>
       <c r="F136" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="28"/>
+        <v>Samsung_TV_soundMode</v>
+      </c>
+      <c r="H136" t="str">
+        <f t="shared" si="29"/>
+        <v>Samsung_TV_soundMode_music:"setSoundMode(ENUM)",</v>
+      </c>
+      <c r="I136" t="str">
+        <f t="shared" si="30"/>
         <v>attributeCommandMap.put("Samsung TV_soundMode_music","setSoundMode(ENUM)");</v>
       </c>
     </row>
-    <row r="137" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>168</v>
       </c>
@@ -5052,11 +5668,19 @@
         <v>295</v>
       </c>
       <c r="F137" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="28"/>
+        <v>Samsung_TV_soundMode</v>
+      </c>
+      <c r="H137" t="str">
+        <f t="shared" si="29"/>
+        <v>Samsung_TV_soundMode_standard:"setSoundMode(ENUM)",</v>
+      </c>
+      <c r="I137" t="str">
+        <f t="shared" si="30"/>
         <v>attributeCommandMap.put("Samsung TV_soundMode_standard","setSoundMode(ENUM)");</v>
       </c>
     </row>
-    <row r="138" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>168</v>
       </c>
@@ -5073,11 +5697,19 @@
         <v>295</v>
       </c>
       <c r="F138" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="28"/>
+        <v>Samsung_TV_soundMode</v>
+      </c>
+      <c r="H138" t="str">
+        <f t="shared" si="29"/>
+        <v>Samsung_TV_soundMode_unknown:"setSoundMode(ENUM)",</v>
+      </c>
+      <c r="I138" t="str">
+        <f t="shared" si="30"/>
         <v>attributeCommandMap.put("Samsung TV_soundMode_unknown","setSoundMode(ENUM)");</v>
       </c>
     </row>
-    <row r="139" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>168</v>
       </c>
@@ -5094,11 +5726,22 @@
         <v>5</v>
       </c>
       <c r="F139" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="F139:F141" si="31">CONCATENATE(SUBSTITUTE(A139," ","_"),"_",B139)</f>
+        <v>Samsung_TV_switch</v>
+      </c>
+      <c r="G139" t="s">
+        <v>111</v>
+      </c>
+      <c r="H139" t="str">
+        <f t="shared" si="29"/>
+        <v>Samsung_TV_switch_off:"off()",</v>
+      </c>
+      <c r="I139" t="str">
+        <f t="shared" si="30"/>
         <v>attributeCommandMap.put("Samsung TV_switch_off","off()");</v>
       </c>
     </row>
-    <row r="140" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>168</v>
       </c>
@@ -5115,11 +5758,22 @@
         <v>92</v>
       </c>
       <c r="F140" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="31"/>
+        <v>Samsung_TV_switch</v>
+      </c>
+      <c r="G140" t="s">
+        <v>111</v>
+      </c>
+      <c r="H140" t="str">
+        <f t="shared" si="29"/>
+        <v>Samsung_TV_switch_on:"on()",</v>
+      </c>
+      <c r="I140" t="str">
+        <f t="shared" si="30"/>
         <v>attributeCommandMap.put("Samsung TV_switch_on","on()");</v>
       </c>
     </row>
-    <row r="141" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>168</v>
       </c>
@@ -5133,11 +5787,22 @@
         <v>296</v>
       </c>
       <c r="F141" t="str">
+        <f t="shared" si="31"/>
+        <v>Samsung_TV_volume</v>
+      </c>
+      <c r="G141" t="s">
+        <v>311</v>
+      </c>
+      <c r="H141" t="str">
+        <f t="shared" si="29"/>
+        <v>Samsung_TV_volume:"setVolume(NUMBER)",</v>
+      </c>
+      <c r="I141" t="str">
         <f>CONCATENATE("attributeCommandMap.put(""",A141,"_",B141,""",""","",E141,""");")</f>
         <v>attributeCommandMap.put("Samsung TV_volume","setVolume(NUMBER)");</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>168</v>
       </c>
@@ -5145,7 +5810,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>168</v>
       </c>
@@ -5153,7 +5818,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>168</v>
       </c>
@@ -5161,7 +5826,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="145" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>94</v>
       </c>
@@ -5174,8 +5839,15 @@
       <c r="D145" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="146" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F145" t="str">
+        <f t="shared" ref="F145:F148" si="32">CONCATENATE(SUBSTITUTE(A145," ","_"),"_",B145)</f>
+        <v>Shock_Sensor_shock</v>
+      </c>
+      <c r="G145" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>94</v>
       </c>
@@ -5188,8 +5860,15 @@
       <c r="D146" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="147" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F146" t="str">
+        <f t="shared" si="32"/>
+        <v>Shock_Sensor_shock</v>
+      </c>
+      <c r="G146" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>96</v>
       </c>
@@ -5199,8 +5878,15 @@
       <c r="C147" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="148" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F147" t="str">
+        <f t="shared" si="32"/>
+        <v>Signal_Strength_lqi</v>
+      </c>
+      <c r="G147" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>96</v>
       </c>
@@ -5210,8 +5896,15 @@
       <c r="C148" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="149" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F148" t="str">
+        <f t="shared" si="32"/>
+        <v>Signal_Strength_rssi</v>
+      </c>
+      <c r="G148" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>99</v>
       </c>
@@ -5224,8 +5917,15 @@
       <c r="D149" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="150" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F149" t="str">
+        <f t="shared" ref="F149:F154" si="33">CONCATENATE(SUBSTITUTE(A149," ","_"),"_",B149)</f>
+        <v>Sleep_Sensor_sleeping</v>
+      </c>
+      <c r="G149" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>99</v>
       </c>
@@ -5238,8 +5938,15 @@
       <c r="D150" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="151" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F150" t="str">
+        <f t="shared" si="33"/>
+        <v>Sleep_Sensor_sleeping</v>
+      </c>
+      <c r="G150" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>101</v>
       </c>
@@ -5252,8 +5959,12 @@
       <c r="D151" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="152" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F151" t="str">
+        <f t="shared" si="33"/>
+        <v>Smoke_Detector_smoke</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>101</v>
       </c>
@@ -5266,8 +5977,12 @@
       <c r="D152" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="153" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F152" t="str">
+        <f t="shared" si="33"/>
+        <v>Smoke_Detector_smoke</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>101</v>
       </c>
@@ -5280,8 +5995,12 @@
       <c r="D153" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="154" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F153" t="str">
+        <f t="shared" si="33"/>
+        <v>Smoke_Detector_smoke</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>113</v>
       </c>
@@ -5291,8 +6010,15 @@
       <c r="C154" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="155" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F154" t="str">
+        <f t="shared" si="33"/>
+        <v>Sound_Pressure_Level_soundPressureLevel</v>
+      </c>
+      <c r="G154" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>103</v>
       </c>
@@ -5305,8 +6031,15 @@
       <c r="D155" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="156" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F155" t="str">
+        <f t="shared" ref="F155:F160" si="34">CONCATENATE(SUBSTITUTE(A155," ","_"),"_",B155)</f>
+        <v>Sound_Sensor_sound</v>
+      </c>
+      <c r="G155" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>103</v>
       </c>
@@ -5319,8 +6052,15 @@
       <c r="D156" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="157" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F156" t="str">
+        <f t="shared" si="34"/>
+        <v>Sound_Sensor_sound</v>
+      </c>
+      <c r="G156" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>105</v>
       </c>
@@ -5330,8 +6070,12 @@
       <c r="C157" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F157" t="str">
+        <f t="shared" si="34"/>
+        <v>Speech_Recognition_phraseSpoken</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>107</v>
       </c>
@@ -5339,7 +6083,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="159" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>108</v>
       </c>
@@ -5349,8 +6093,15 @@
       <c r="C159" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="160" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F159" t="str">
+        <f t="shared" si="34"/>
+        <v>Step_Sensor_goal</v>
+      </c>
+      <c r="G159" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>108</v>
       </c>
@@ -5360,8 +6111,15 @@
       <c r="C160" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="161" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F160" t="str">
+        <f t="shared" si="34"/>
+        <v>Step_Sensor_steps</v>
+      </c>
+      <c r="G160" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>111</v>
       </c>
@@ -5378,11 +6136,22 @@
         <v>5</v>
       </c>
       <c r="F161" t="str">
-        <f t="shared" ref="F161:F162" si="7">CONCATENATE("attributeCommandMap.put(""",A161,"_",B161,"_",D161,""",""","",E161,""");")</f>
+        <f t="shared" ref="F161:F163" si="35">CONCATENATE(SUBSTITUTE(A161," ","_"),"_",B161)</f>
+        <v>Switch_switch</v>
+      </c>
+      <c r="G161" t="s">
+        <v>111</v>
+      </c>
+      <c r="H161" t="str">
+        <f t="shared" ref="H161:H163" si="36">SUBSTITUTE(CONCATENATE(A161,"_",B161,IF(D161="","",CONCATENATE("_",D161)),":""",E161,""",")," ","_")</f>
+        <v>Switch_switch_off:"off()",</v>
+      </c>
+      <c r="I161" t="str">
+        <f t="shared" ref="I161:I162" si="37">CONCATENATE("attributeCommandMap.put(""",A161,"_",B161,"_",D161,""",""","",E161,""");")</f>
         <v>attributeCommandMap.put("Switch_switch_off","off()");</v>
       </c>
     </row>
-    <row r="162" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>111</v>
       </c>
@@ -5399,11 +6168,22 @@
         <v>92</v>
       </c>
       <c r="F162" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="35"/>
+        <v>Switch_switch</v>
+      </c>
+      <c r="G162" t="s">
+        <v>111</v>
+      </c>
+      <c r="H162" t="str">
+        <f t="shared" si="36"/>
+        <v>Switch_switch_on:"on()",</v>
+      </c>
+      <c r="I162" t="str">
+        <f t="shared" si="37"/>
         <v>attributeCommandMap.put("Switch_switch_on","on()");</v>
       </c>
     </row>
-    <row r="163" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>112</v>
       </c>
@@ -5417,11 +6197,22 @@
         <v>299</v>
       </c>
       <c r="F163" t="str">
+        <f t="shared" si="35"/>
+        <v>Switch_Level_level</v>
+      </c>
+      <c r="G163" t="s">
+        <v>310</v>
+      </c>
+      <c r="H163" t="str">
+        <f t="shared" si="36"/>
+        <v>Switch_Level_level:"setLevel(NUMBER,NUMBER)",</v>
+      </c>
+      <c r="I163" t="str">
         <f>CONCATENATE("attributeCommandMap.put(""",A163,"_",B163,""",""","",E163,""");")</f>
         <v>attributeCommandMap.put("Switch Level_level","setLevel(NUMBER,NUMBER)");</v>
       </c>
     </row>
-    <row r="164" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>115</v>
       </c>
@@ -5434,8 +6225,15 @@
       <c r="D164" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="165" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F164" t="str">
+        <f t="shared" ref="F164:F186" si="38">CONCATENATE(SUBSTITUTE(A164," ","_"),"_",B164)</f>
+        <v>Tamper_Alert_tamper</v>
+      </c>
+      <c r="G164" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>115</v>
       </c>
@@ -5448,8 +6246,15 @@
       <c r="D165" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="166" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F165" t="str">
+        <f t="shared" si="38"/>
+        <v>Tamper_Alert_tamper</v>
+      </c>
+      <c r="G165" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>117</v>
       </c>
@@ -5459,8 +6264,15 @@
       <c r="C166" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="167" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F166" t="str">
+        <f t="shared" si="38"/>
+        <v>Temperature_Measurement_temperature</v>
+      </c>
+      <c r="G166" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>119</v>
       </c>
@@ -5474,11 +6286,22 @@
         <v>300</v>
       </c>
       <c r="F167" t="str">
-        <f t="shared" ref="F167:F168" si="8">CONCATENATE("attributeCommandMap.put(""",A167,"_",B167,""",""","",E167,""");")</f>
+        <f t="shared" si="38"/>
+        <v>Thermostat_coolingSetpoint</v>
+      </c>
+      <c r="G167" t="s">
+        <v>311</v>
+      </c>
+      <c r="H167" t="str">
+        <f t="shared" ref="H167:H168" si="39">SUBSTITUTE(CONCATENATE(A167,"_",B167,IF(D167="","",CONCATENATE("_",D167)),":""",E167,""",")," ","_")</f>
+        <v>Thermostat_coolingSetpoint:"setCoolingSetpoint(NUMBER)",</v>
+      </c>
+      <c r="I167" t="str">
+        <f t="shared" ref="I167:I168" si="40">CONCATENATE("attributeCommandMap.put(""",A167,"_",B167,""",""","",E167,""");")</f>
         <v>attributeCommandMap.put("Thermostat_coolingSetpoint","setCoolingSetpoint(NUMBER)");</v>
       </c>
     </row>
-    <row r="168" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>119</v>
       </c>
@@ -5492,11 +6315,22 @@
         <v>301</v>
       </c>
       <c r="F168" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="38"/>
+        <v>Thermostat_heatingSetpoint</v>
+      </c>
+      <c r="G168" t="s">
+        <v>311</v>
+      </c>
+      <c r="H168" t="str">
+        <f t="shared" si="39"/>
+        <v>Thermostat_heatingSetpoint:"setHeatingSetpoint(NUMBER)",</v>
+      </c>
+      <c r="I168" t="str">
+        <f t="shared" si="40"/>
         <v>attributeCommandMap.put("Thermostat_heatingSetpoint","setHeatingSetpoint(NUMBER)");</v>
       </c>
     </row>
-    <row r="169" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>119</v>
       </c>
@@ -5506,8 +6340,12 @@
       <c r="C169" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="170" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F169" t="str">
+        <f t="shared" si="38"/>
+        <v>Thermostat_schedule</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>119</v>
       </c>
@@ -5517,8 +6355,15 @@
       <c r="C170" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="171" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F170" t="str">
+        <f t="shared" si="38"/>
+        <v>Thermostat_temperature</v>
+      </c>
+      <c r="G170" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>119</v>
       </c>
@@ -5535,11 +6380,19 @@
         <v>130</v>
       </c>
       <c r="F171" t="str">
-        <f t="shared" ref="F171:F178" si="9">CONCATENATE("attributeCommandMap.put(""",A171,"_",B171,"_",D171,""",""","",E171,""");")</f>
+        <f t="shared" si="38"/>
+        <v>Thermostat_thermostatFanMode</v>
+      </c>
+      <c r="H171" t="str">
+        <f t="shared" ref="H171:H178" si="41">SUBSTITUTE(CONCATENATE(A171,"_",B171,IF(D171="","",CONCATENATE("_",D171)),":""",E171,""",")," ","_")</f>
+        <v>Thermostat_thermostatFanMode_auto:"fanAuto()",</v>
+      </c>
+      <c r="I171" t="str">
+        <f t="shared" ref="I171:I178" si="42">CONCATENATE("attributeCommandMap.put(""",A171,"_",B171,"_",D171,""",""","",E171,""");")</f>
         <v>attributeCommandMap.put("Thermostat_thermostatFanMode_auto","fanAuto()");</v>
       </c>
     </row>
-    <row r="172" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>119</v>
       </c>
@@ -5556,11 +6409,19 @@
         <v>131</v>
       </c>
       <c r="F172" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="38"/>
+        <v>Thermostat_thermostatFanMode</v>
+      </c>
+      <c r="H172" t="str">
+        <f t="shared" si="41"/>
+        <v>Thermostat_thermostatFanMode_circulate:"fanCirculate()",</v>
+      </c>
+      <c r="I172" t="str">
+        <f t="shared" si="42"/>
         <v>attributeCommandMap.put("Thermostat_thermostatFanMode_circulate","fanCirculate()");</v>
       </c>
     </row>
-    <row r="173" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>119</v>
       </c>
@@ -5577,11 +6438,19 @@
         <v>129</v>
       </c>
       <c r="F173" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="38"/>
+        <v>Thermostat_thermostatFanMode</v>
+      </c>
+      <c r="H173" t="str">
+        <f t="shared" si="41"/>
+        <v>Thermostat_thermostatFanMode_on:"fanOn()",</v>
+      </c>
+      <c r="I173" t="str">
+        <f t="shared" si="42"/>
         <v>attributeCommandMap.put("Thermostat_thermostatFanMode_on","fanOn()");</v>
       </c>
     </row>
-    <row r="174" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>119</v>
       </c>
@@ -5598,11 +6467,19 @@
         <v>132</v>
       </c>
       <c r="F174" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="38"/>
+        <v>Thermostat_thermostatMode</v>
+      </c>
+      <c r="H174" t="str">
+        <f t="shared" si="41"/>
+        <v>Thermostat_thermostatMode_auto:"auto()",</v>
+      </c>
+      <c r="I174" t="str">
+        <f t="shared" si="42"/>
         <v>attributeCommandMap.put("Thermostat_thermostatMode_auto","auto()");</v>
       </c>
     </row>
-    <row r="175" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>119</v>
       </c>
@@ -5619,11 +6496,19 @@
         <v>128</v>
       </c>
       <c r="F175" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="38"/>
+        <v>Thermostat_thermostatMode</v>
+      </c>
+      <c r="H175" t="str">
+        <f t="shared" si="41"/>
+        <v>Thermostat_thermostatMode_cool:"cool()",</v>
+      </c>
+      <c r="I175" t="str">
+        <f t="shared" si="42"/>
         <v>attributeCommandMap.put("Thermostat_thermostatMode_cool","cool()");</v>
       </c>
     </row>
-    <row r="176" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>119</v>
       </c>
@@ -5640,11 +6525,19 @@
         <v>127</v>
       </c>
       <c r="F176" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="38"/>
+        <v>Thermostat_thermostatMode</v>
+      </c>
+      <c r="H176" t="str">
+        <f t="shared" si="41"/>
+        <v>Thermostat_thermostatMode_emergency_heat:"emergencyHeat()",</v>
+      </c>
+      <c r="I176" t="str">
+        <f t="shared" si="42"/>
         <v>attributeCommandMap.put("Thermostat_thermostatMode_emergency heat","emergencyHeat()");</v>
       </c>
     </row>
-    <row r="177" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>119</v>
       </c>
@@ -5661,11 +6554,19 @@
         <v>126</v>
       </c>
       <c r="F177" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="38"/>
+        <v>Thermostat_thermostatMode</v>
+      </c>
+      <c r="H177" t="str">
+        <f t="shared" si="41"/>
+        <v>Thermostat_thermostatMode_heat:"heat()",</v>
+      </c>
+      <c r="I177" t="str">
+        <f t="shared" si="42"/>
         <v>attributeCommandMap.put("Thermostat_thermostatMode_heat","heat()");</v>
       </c>
     </row>
-    <row r="178" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>119</v>
       </c>
@@ -5682,11 +6583,19 @@
         <v>5</v>
       </c>
       <c r="F178" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="38"/>
+        <v>Thermostat_thermostatMode</v>
+      </c>
+      <c r="H178" t="str">
+        <f t="shared" si="41"/>
+        <v>Thermostat_thermostatMode_off:"off()",</v>
+      </c>
+      <c r="I178" t="str">
+        <f t="shared" si="42"/>
         <v>attributeCommandMap.put("Thermostat_thermostatMode_off","off()");</v>
       </c>
     </row>
-    <row r="179" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>119</v>
       </c>
@@ -5699,8 +6608,12 @@
       <c r="D179" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="180" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F179" t="str">
+        <f t="shared" si="38"/>
+        <v>Thermostat_thermostatOperatingState</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>119</v>
       </c>
@@ -5713,8 +6626,12 @@
       <c r="D180" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="181" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F180" t="str">
+        <f t="shared" si="38"/>
+        <v>Thermostat_thermostatOperatingState</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>119</v>
       </c>
@@ -5727,8 +6644,12 @@
       <c r="D181" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="182" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F181" t="str">
+        <f t="shared" si="38"/>
+        <v>Thermostat_thermostatOperatingState</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>119</v>
       </c>
@@ -5741,8 +6662,12 @@
       <c r="D182" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="183" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F182" t="str">
+        <f t="shared" si="38"/>
+        <v>Thermostat_thermostatOperatingState</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>119</v>
       </c>
@@ -5755,8 +6680,12 @@
       <c r="D183" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="184" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F183" t="str">
+        <f t="shared" si="38"/>
+        <v>Thermostat_thermostatOperatingState</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>119</v>
       </c>
@@ -5769,8 +6698,12 @@
       <c r="D184" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="185" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F184" t="str">
+        <f t="shared" si="38"/>
+        <v>Thermostat_thermostatOperatingState</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>119</v>
       </c>
@@ -5783,8 +6716,12 @@
       <c r="D185" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="186" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F185" t="str">
+        <f t="shared" si="38"/>
+        <v>Thermostat_thermostatOperatingState</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>119</v>
       </c>
@@ -5794,8 +6731,15 @@
       <c r="C186" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F186" t="str">
+        <f t="shared" si="38"/>
+        <v>Thermostat_thermostatSetpoint</v>
+      </c>
+      <c r="G186" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>119</v>
       </c>
@@ -5803,7 +6747,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>119</v>
       </c>
@@ -5811,7 +6755,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>119</v>
       </c>
@@ -5819,7 +6763,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="190" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>133</v>
       </c>
@@ -5833,11 +6777,22 @@
         <v>300</v>
       </c>
       <c r="F190" t="str">
+        <f t="shared" ref="F190:F193" si="43">CONCATENATE(SUBSTITUTE(A190," ","_"),"_",B190)</f>
+        <v>Thermostat_Cooling_Setpoint_coolingSetpoint</v>
+      </c>
+      <c r="G190" t="s">
+        <v>311</v>
+      </c>
+      <c r="H190" t="str">
+        <f t="shared" ref="H190:H193" si="44">SUBSTITUTE(CONCATENATE(A190,"_",B190,IF(D190="","",CONCATENATE("_",D190)),":""",E190,""",")," ","_")</f>
+        <v>Thermostat_Cooling_Setpoint_coolingSetpoint:"setCoolingSetpoint(NUMBER)",</v>
+      </c>
+      <c r="I190" t="str">
         <f>CONCATENATE("attributeCommandMap.put(""",A190,"_",B190,""",""","",E190,""");")</f>
         <v>attributeCommandMap.put("Thermostat Cooling Setpoint_coolingSetpoint","setCoolingSetpoint(NUMBER)");</v>
       </c>
     </row>
-    <row r="191" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>134</v>
       </c>
@@ -5854,11 +6809,19 @@
         <v>130</v>
       </c>
       <c r="F191" t="str">
-        <f t="shared" ref="F191:F193" si="10">CONCATENATE("attributeCommandMap.put(""",A191,"_",B191,"_",D191,""",""","",E191,""");")</f>
+        <f t="shared" si="43"/>
+        <v>Thermostat_Fan_Mode_thermostatFanMode</v>
+      </c>
+      <c r="H191" t="str">
+        <f t="shared" si="44"/>
+        <v>Thermostat_Fan_Mode_thermostatFanMode_auto:"fanAuto()",</v>
+      </c>
+      <c r="I191" t="str">
+        <f t="shared" ref="I191:I193" si="45">CONCATENATE("attributeCommandMap.put(""",A191,"_",B191,"_",D191,""",""","",E191,""");")</f>
         <v>attributeCommandMap.put("Thermostat Fan Mode_thermostatFanMode_auto","fanAuto()");</v>
       </c>
     </row>
-    <row r="192" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>134</v>
       </c>
@@ -5875,11 +6838,19 @@
         <v>131</v>
       </c>
       <c r="F192" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="43"/>
+        <v>Thermostat_Fan_Mode_thermostatFanMode</v>
+      </c>
+      <c r="H192" t="str">
+        <f t="shared" si="44"/>
+        <v>Thermostat_Fan_Mode_thermostatFanMode_circulate:"fanCirculate()",</v>
+      </c>
+      <c r="I192" t="str">
+        <f t="shared" si="45"/>
         <v>attributeCommandMap.put("Thermostat Fan Mode_thermostatFanMode_circulate","fanCirculate()");</v>
       </c>
     </row>
-    <row r="193" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>134</v>
       </c>
@@ -5896,11 +6867,19 @@
         <v>129</v>
       </c>
       <c r="F193" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="43"/>
+        <v>Thermostat_Fan_Mode_thermostatFanMode</v>
+      </c>
+      <c r="H193" t="str">
+        <f t="shared" si="44"/>
+        <v>Thermostat_Fan_Mode_thermostatFanMode_on:"fanOn()",</v>
+      </c>
+      <c r="I193" t="str">
+        <f t="shared" si="45"/>
         <v>attributeCommandMap.put("Thermostat Fan Mode_thermostatFanMode_on","fanOn()");</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>134</v>
       </c>
@@ -5908,7 +6887,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="195" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>135</v>
       </c>
@@ -5922,11 +6901,22 @@
         <v>301</v>
       </c>
       <c r="F195" t="str">
+        <f t="shared" ref="F195:F200" si="46">CONCATENATE(SUBSTITUTE(A195," ","_"),"_",B195)</f>
+        <v>Thermostat_Heating_Setpoint_heatingSetpoint</v>
+      </c>
+      <c r="G195" t="s">
+        <v>311</v>
+      </c>
+      <c r="H195" t="str">
+        <f t="shared" ref="H195:H200" si="47">SUBSTITUTE(CONCATENATE(A195,"_",B195,IF(D195="","",CONCATENATE("_",D195)),":""",E195,""",")," ","_")</f>
+        <v>Thermostat_Heating_Setpoint_heatingSetpoint:"setHeatingSetpoint(NUMBER)",</v>
+      </c>
+      <c r="I195" t="str">
         <f>CONCATENATE("attributeCommandMap.put(""",A195,"_",B195,""",""","",E195,""");")</f>
         <v>attributeCommandMap.put("Thermostat Heating Setpoint_heatingSetpoint","setHeatingSetpoint(NUMBER)");</v>
       </c>
     </row>
-    <row r="196" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>136</v>
       </c>
@@ -5943,11 +6933,19 @@
         <v>132</v>
       </c>
       <c r="F196" t="str">
-        <f t="shared" ref="F196:F200" si="11">CONCATENATE("attributeCommandMap.put(""",A196,"_",B196,"_",D196,""",""","",E196,""");")</f>
+        <f t="shared" si="46"/>
+        <v>Thermostat_Mode_thermostatMode</v>
+      </c>
+      <c r="H196" t="str">
+        <f t="shared" si="47"/>
+        <v>Thermostat_Mode_thermostatMode_auto:"auto()",</v>
+      </c>
+      <c r="I196" t="str">
+        <f t="shared" ref="I196:I200" si="48">CONCATENATE("attributeCommandMap.put(""",A196,"_",B196,"_",D196,""",""","",E196,""");")</f>
         <v>attributeCommandMap.put("Thermostat Mode_thermostatMode_auto","auto()");</v>
       </c>
     </row>
-    <row r="197" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>136</v>
       </c>
@@ -5964,11 +6962,19 @@
         <v>128</v>
       </c>
       <c r="F197" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="46"/>
+        <v>Thermostat_Mode_thermostatMode</v>
+      </c>
+      <c r="H197" t="str">
+        <f t="shared" si="47"/>
+        <v>Thermostat_Mode_thermostatMode_cool:"cool()",</v>
+      </c>
+      <c r="I197" t="str">
+        <f t="shared" si="48"/>
         <v>attributeCommandMap.put("Thermostat Mode_thermostatMode_cool","cool()");</v>
       </c>
     </row>
-    <row r="198" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>136</v>
       </c>
@@ -5985,11 +6991,19 @@
         <v>127</v>
       </c>
       <c r="F198" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="46"/>
+        <v>Thermostat_Mode_thermostatMode</v>
+      </c>
+      <c r="H198" t="str">
+        <f t="shared" si="47"/>
+        <v>Thermostat_Mode_thermostatMode_emergency_heat:"emergencyHeat()",</v>
+      </c>
+      <c r="I198" t="str">
+        <f t="shared" si="48"/>
         <v>attributeCommandMap.put("Thermostat Mode_thermostatMode_emergency heat","emergencyHeat()");</v>
       </c>
     </row>
-    <row r="199" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>136</v>
       </c>
@@ -6006,11 +7020,19 @@
         <v>126</v>
       </c>
       <c r="F199" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="46"/>
+        <v>Thermostat_Mode_thermostatMode</v>
+      </c>
+      <c r="H199" t="str">
+        <f t="shared" si="47"/>
+        <v>Thermostat_Mode_thermostatMode_heat:"heat()",</v>
+      </c>
+      <c r="I199" t="str">
+        <f t="shared" si="48"/>
         <v>attributeCommandMap.put("Thermostat Mode_thermostatMode_heat","heat()");</v>
       </c>
     </row>
-    <row r="200" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>136</v>
       </c>
@@ -6027,11 +7049,19 @@
         <v>5</v>
       </c>
       <c r="F200" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="46"/>
+        <v>Thermostat_Mode_thermostatMode</v>
+      </c>
+      <c r="H200" t="str">
+        <f t="shared" si="47"/>
+        <v>Thermostat_Mode_thermostatMode_off:"off()",</v>
+      </c>
+      <c r="I200" t="str">
+        <f t="shared" si="48"/>
         <v>attributeCommandMap.put("Thermostat Mode_thermostatMode_off","off()");</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>136</v>
       </c>
@@ -6039,7 +7069,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="202" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>137</v>
       </c>
@@ -6052,8 +7082,12 @@
       <c r="D202" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="203" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F202" t="str">
+        <f t="shared" ref="F202:F216" si="49">CONCATENATE(SUBSTITUTE(A202," ","_"),"_",B202)</f>
+        <v>Thermostat_Operating_State_thermostatOperatingState</v>
+      </c>
+    </row>
+    <row r="203" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>137</v>
       </c>
@@ -6066,8 +7100,12 @@
       <c r="D203" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="204" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F203" t="str">
+        <f t="shared" si="49"/>
+        <v>Thermostat_Operating_State_thermostatOperatingState</v>
+      </c>
+    </row>
+    <row r="204" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>137</v>
       </c>
@@ -6080,8 +7118,12 @@
       <c r="D204" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="205" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F204" t="str">
+        <f t="shared" si="49"/>
+        <v>Thermostat_Operating_State_thermostatOperatingState</v>
+      </c>
+    </row>
+    <row r="205" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>137</v>
       </c>
@@ -6094,8 +7136,12 @@
       <c r="D205" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="206" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F205" t="str">
+        <f t="shared" si="49"/>
+        <v>Thermostat_Operating_State_thermostatOperatingState</v>
+      </c>
+    </row>
+    <row r="206" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>137</v>
       </c>
@@ -6108,8 +7154,12 @@
       <c r="D206" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="207" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F206" t="str">
+        <f t="shared" si="49"/>
+        <v>Thermostat_Operating_State_thermostatOperatingState</v>
+      </c>
+    </row>
+    <row r="207" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>137</v>
       </c>
@@ -6122,8 +7172,12 @@
       <c r="D207" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="208" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F207" t="str">
+        <f t="shared" si="49"/>
+        <v>Thermostat_Operating_State_thermostatOperatingState</v>
+      </c>
+    </row>
+    <row r="208" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>137</v>
       </c>
@@ -6136,8 +7190,12 @@
       <c r="D208" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="209" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F208" t="str">
+        <f t="shared" si="49"/>
+        <v>Thermostat_Operating_State_thermostatOperatingState</v>
+      </c>
+    </row>
+    <row r="209" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>161</v>
       </c>
@@ -6151,11 +7209,19 @@
         <v>302</v>
       </c>
       <c r="F209" t="str">
+        <f t="shared" si="49"/>
+        <v>Thermostat_Schedule_schedule</v>
+      </c>
+      <c r="H209" t="str">
+        <f>SUBSTITUTE(CONCATENATE(A209,"_",B209,IF(D209="","",CONCATENATE("_",D209)),":""",E209,""",")," ","_")</f>
+        <v>Thermostat_Schedule_schedule:"setSchedule(JSON_OBJECT)",</v>
+      </c>
+      <c r="I209" t="str">
         <f>CONCATENATE("attributeCommandMap.put(""",A209,"_",B209,""",""","",E209,""");")</f>
         <v>attributeCommandMap.put("Thermostat Schedule_schedule","setSchedule(JSON_OBJECT)");</v>
       </c>
     </row>
-    <row r="210" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>138</v>
       </c>
@@ -6165,8 +7231,15 @@
       <c r="C210" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="211" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F210" t="str">
+        <f t="shared" si="49"/>
+        <v>Thermostat_Setpoint_thermostatSetpoint</v>
+      </c>
+      <c r="G210" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="211" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>139</v>
       </c>
@@ -6176,8 +7249,12 @@
       <c r="C211" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="212" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F211" t="str">
+        <f t="shared" si="49"/>
+        <v>Three_Axis_threeAxis</v>
+      </c>
+    </row>
+    <row r="212" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>141</v>
       </c>
@@ -6194,11 +7271,19 @@
         <v>145</v>
       </c>
       <c r="F212" t="str">
-        <f t="shared" ref="F212:F215" si="12">CONCATENATE("attributeCommandMap.put(""",A212,"_",B212,"_",D212,""",""","",E212,""");")</f>
+        <f t="shared" si="49"/>
+        <v>Timed_Session_sessionStatus</v>
+      </c>
+      <c r="H212" t="str">
+        <f t="shared" ref="H212:H216" si="50">SUBSTITUTE(CONCATENATE(A212,"_",B212,IF(D212="","",CONCATENATE("_",D212)),":""",E212,""",")," ","_")</f>
+        <v>Timed_Session_sessionStatus_canceled:"cancel()",</v>
+      </c>
+      <c r="I212" t="str">
+        <f t="shared" ref="I212:I215" si="51">CONCATENATE("attributeCommandMap.put(""",A212,"_",B212,"_",D212,""",""","",E212,""");")</f>
         <v>attributeCommandMap.put("Timed Session_sessionStatus_canceled","cancel()");</v>
       </c>
     </row>
-    <row r="213" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>141</v>
       </c>
@@ -6215,11 +7300,19 @@
         <v>70</v>
       </c>
       <c r="F213" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="49"/>
+        <v>Timed_Session_sessionStatus</v>
+      </c>
+      <c r="H213" t="str">
+        <f t="shared" si="50"/>
+        <v>Timed_Session_sessionStatus_paused:"pause()",</v>
+      </c>
+      <c r="I213" t="str">
+        <f t="shared" si="51"/>
         <v>attributeCommandMap.put("Timed Session_sessionStatus_paused","pause()");</v>
       </c>
     </row>
-    <row r="214" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>141</v>
       </c>
@@ -6236,11 +7329,19 @@
         <v>144</v>
       </c>
       <c r="F214" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="49"/>
+        <v>Timed_Session_sessionStatus</v>
+      </c>
+      <c r="H214" t="str">
+        <f t="shared" si="50"/>
+        <v>Timed_Session_sessionStatus_running:"start()",</v>
+      </c>
+      <c r="I214" t="str">
+        <f t="shared" si="51"/>
         <v>attributeCommandMap.put("Timed Session_sessionStatus_running","start()");</v>
       </c>
     </row>
-    <row r="215" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>141</v>
       </c>
@@ -6257,11 +7358,19 @@
         <v>71</v>
       </c>
       <c r="F215" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="49"/>
+        <v>Timed_Session_sessionStatus</v>
+      </c>
+      <c r="H215" t="str">
+        <f t="shared" si="50"/>
+        <v>Timed_Session_sessionStatus_stopped:"stop()",</v>
+      </c>
+      <c r="I215" t="str">
+        <f t="shared" si="51"/>
         <v>attributeCommandMap.put("Timed Session_sessionStatus_stopped","stop()");</v>
       </c>
     </row>
-    <row r="216" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>141</v>
       </c>
@@ -6275,11 +7384,22 @@
         <v>305</v>
       </c>
       <c r="F216" t="str">
+        <f t="shared" si="49"/>
+        <v>Timed_Session_timeRemaining</v>
+      </c>
+      <c r="G216" t="s">
+        <v>311</v>
+      </c>
+      <c r="H216" t="str">
+        <f t="shared" si="50"/>
+        <v>Timed_Session_timeRemaining:"setTimeRemaining(NUMBER)",</v>
+      </c>
+      <c r="I216" t="str">
         <f>CONCATENATE("attributeCommandMap.put(""",A216,"_",B216,""",""","",E216,""");")</f>
         <v>attributeCommandMap.put("Timed Session_timeRemaining","setTimeRemaining(NUMBER)");</v>
       </c>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>146</v>
       </c>
@@ -6287,7 +7407,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="218" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>148</v>
       </c>
@@ -6300,8 +7420,12 @@
       <c r="D218" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="219" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F218" t="str">
+        <f t="shared" ref="F218:F224" si="52">CONCATENATE(SUBSTITUTE(A218," ","_"),"_",B218)</f>
+        <v>Touch_Sensor_touch</v>
+      </c>
+    </row>
+    <row r="219" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>167</v>
       </c>
@@ -6311,8 +7435,15 @@
       <c r="C219" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="220" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F219" t="str">
+        <f t="shared" si="52"/>
+        <v>TV_channel</v>
+      </c>
+      <c r="G219" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="220" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>167</v>
       </c>
@@ -6322,8 +7453,12 @@
       <c r="C220" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="221" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F220" t="str">
+        <f t="shared" si="52"/>
+        <v>TV_movieMode</v>
+      </c>
+    </row>
+    <row r="221" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>167</v>
       </c>
@@ -6333,8 +7468,12 @@
       <c r="C221" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="222" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F221" t="str">
+        <f t="shared" si="52"/>
+        <v>TV_picture</v>
+      </c>
+    </row>
+    <row r="222" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>167</v>
       </c>
@@ -6344,8 +7483,12 @@
       <c r="C222" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="223" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F222" t="str">
+        <f t="shared" si="52"/>
+        <v>TV_power</v>
+      </c>
+    </row>
+    <row r="223" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>167</v>
       </c>
@@ -6355,8 +7498,12 @@
       <c r="C223" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="224" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F223" t="str">
+        <f t="shared" si="52"/>
+        <v>TV_sound</v>
+      </c>
+    </row>
+    <row r="224" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>167</v>
       </c>
@@ -6366,8 +7513,15 @@
       <c r="C224" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F224" t="str">
+        <f t="shared" si="52"/>
+        <v>TV_volume</v>
+      </c>
+      <c r="G224" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>167</v>
       </c>
@@ -6375,7 +7529,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>167</v>
       </c>
@@ -6383,7 +7537,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>167</v>
       </c>
@@ -6391,7 +7545,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>167</v>
       </c>
@@ -6399,7 +7553,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="229" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>150</v>
       </c>
@@ -6409,8 +7563,15 @@
       <c r="C229" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="230" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F229" t="str">
+        <f t="shared" ref="F229" si="53">CONCATENATE(SUBSTITUTE(A229," ","_"),"_",B229)</f>
+        <v>Ultraviolet_Index_ultravioletIndex</v>
+      </c>
+      <c r="G229" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="230" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>152</v>
       </c>
@@ -6423,8 +7584,15 @@
       <c r="D230" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="231" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F230" t="str">
+        <f t="shared" ref="F230:F237" si="54">CONCATENATE(SUBSTITUTE(A230," ","_"),"_",B230)</f>
+        <v>Valve_contact</v>
+      </c>
+      <c r="G230" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="231" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>152</v>
       </c>
@@ -6437,8 +7605,15 @@
       <c r="D231" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="232" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F231" t="str">
+        <f t="shared" si="54"/>
+        <v>Valve_contact</v>
+      </c>
+      <c r="G231" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="232" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>152</v>
       </c>
@@ -6455,11 +7630,22 @@
         <v>35</v>
       </c>
       <c r="F232" t="str">
-        <f t="shared" ref="F232:F235" si="13">CONCATENATE("attributeCommandMap.put(""",A232,"_",B232,"_",D232,""",""","",E232,""");")</f>
+        <f t="shared" si="54"/>
+        <v>Valve_valve</v>
+      </c>
+      <c r="G232" t="s">
+        <v>111</v>
+      </c>
+      <c r="H232" t="str">
+        <f t="shared" ref="H232:H235" si="55">SUBSTITUTE(CONCATENATE(A232,"_",B232,IF(D232="","",CONCATENATE("_",D232)),":""",E232,""",")," ","_")</f>
+        <v>Valve_valve_closed:"close()",</v>
+      </c>
+      <c r="I232" t="str">
+        <f t="shared" ref="I232:I235" si="56">CONCATENATE("attributeCommandMap.put(""",A232,"_",B232,"_",D232,""",""","",E232,""");")</f>
         <v>attributeCommandMap.put("Valve_valve_closed","close()");</v>
       </c>
     </row>
-    <row r="233" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>152</v>
       </c>
@@ -6476,11 +7662,22 @@
         <v>34</v>
       </c>
       <c r="F233" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="54"/>
+        <v>Valve_valve</v>
+      </c>
+      <c r="G233" t="s">
+        <v>111</v>
+      </c>
+      <c r="H233" t="str">
+        <f t="shared" si="55"/>
+        <v>Valve_valve_open:"open()",</v>
+      </c>
+      <c r="I233" t="str">
+        <f t="shared" si="56"/>
         <v>attributeCommandMap.put("Valve_valve_open","open()");</v>
       </c>
     </row>
-    <row r="234" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>160</v>
       </c>
@@ -6497,11 +7694,19 @@
         <v>5</v>
       </c>
       <c r="F234" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="54"/>
+        <v>Video_Camera_camera</v>
+      </c>
+      <c r="H234" t="str">
+        <f t="shared" si="55"/>
+        <v>Video_Camera_camera_off:"off()",</v>
+      </c>
+      <c r="I234" t="str">
+        <f t="shared" si="56"/>
         <v>attributeCommandMap.put("Video Camera_camera_off","off()");</v>
       </c>
     </row>
-    <row r="235" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>160</v>
       </c>
@@ -6518,11 +7723,19 @@
         <v>92</v>
       </c>
       <c r="F235" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="54"/>
+        <v>Video_Camera_camera</v>
+      </c>
+      <c r="H235" t="str">
+        <f t="shared" si="55"/>
+        <v>Video_Camera_camera_on:"on()",</v>
+      </c>
+      <c r="I235" t="str">
+        <f t="shared" si="56"/>
         <v>attributeCommandMap.put("Video Camera_camera_on","on()");</v>
       </c>
     </row>
-    <row r="236" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>160</v>
       </c>
@@ -6535,8 +7748,12 @@
       <c r="D236" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="237" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F236" t="str">
+        <f t="shared" si="54"/>
+        <v>Video_Camera_camera</v>
+      </c>
+    </row>
+    <row r="237" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>160</v>
       </c>
@@ -6549,8 +7766,12 @@
       <c r="D237" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="238" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F237" t="str">
+        <f t="shared" si="54"/>
+        <v>Video_Camera_camera</v>
+      </c>
+    </row>
+    <row r="238" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>160</v>
       </c>
@@ -6567,11 +7788,22 @@
         <v>73</v>
       </c>
       <c r="F238" t="str">
-        <f t="shared" ref="F238:F239" si="14">CONCATENATE("attributeCommandMap.put(""",A238,"_",B238,"_",D238,""",""","",E238,""");")</f>
+        <f t="shared" ref="F238:F245" si="57">CONCATENATE(SUBSTITUTE(A238," ","_"),"_",B238)</f>
+        <v>Video_Camera_mute</v>
+      </c>
+      <c r="G238" t="s">
+        <v>111</v>
+      </c>
+      <c r="H238" t="str">
+        <f t="shared" ref="H238:H239" si="58">SUBSTITUTE(CONCATENATE(A238,"_",B238,IF(D238="","",CONCATENATE("_",D238)),":""",E238,""",")," ","_")</f>
+        <v>Video_Camera_mute_muted:"mute()",</v>
+      </c>
+      <c r="I238" t="str">
+        <f t="shared" ref="I238:I239" si="59">CONCATENATE("attributeCommandMap.put(""",A238,"_",B238,"_",D238,""",""","",E238,""");")</f>
         <v>attributeCommandMap.put("Video Camera_mute_muted","mute()");</v>
       </c>
     </row>
-    <row r="239" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>160</v>
       </c>
@@ -6588,11 +7820,22 @@
         <v>75</v>
       </c>
       <c r="F239" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="57"/>
+        <v>Video_Camera_mute</v>
+      </c>
+      <c r="G239" t="s">
+        <v>111</v>
+      </c>
+      <c r="H239" t="str">
+        <f t="shared" si="58"/>
+        <v>Video_Camera_mute_unmuted:"unmute()",</v>
+      </c>
+      <c r="I239" t="str">
+        <f t="shared" si="59"/>
         <v>attributeCommandMap.put("Video Camera_mute_unmuted","unmute()");</v>
       </c>
     </row>
-    <row r="240" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>160</v>
       </c>
@@ -6602,8 +7845,12 @@
       <c r="C240" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="241" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F240" t="str">
+        <f t="shared" si="57"/>
+        <v>Video_Camera_settings</v>
+      </c>
+    </row>
+    <row r="241" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>160</v>
       </c>
@@ -6613,8 +7860,12 @@
       <c r="C241" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F241" t="str">
+        <f t="shared" si="57"/>
+        <v>Video_Camera_statusMessage</v>
+      </c>
+    </row>
+    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>160</v>
       </c>
@@ -6622,7 +7873,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="243" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>169</v>
       </c>
@@ -6632,8 +7883,12 @@
       <c r="C243" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F243" t="str">
+        <f t="shared" si="57"/>
+        <v>Video_Capture_clip</v>
+      </c>
+    </row>
+    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>169</v>
       </c>
@@ -6641,7 +7896,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="245" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>153</v>
       </c>
@@ -6651,8 +7906,15 @@
       <c r="C245" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="246" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F245" t="str">
+        <f t="shared" si="57"/>
+        <v>Voltage_Measurement_voltage</v>
+      </c>
+      <c r="G245" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="246" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>155</v>
       </c>
@@ -6665,8 +7927,15 @@
       <c r="D246" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="247" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F246" t="str">
+        <f t="shared" ref="F246:F256" si="60">CONCATENATE(SUBSTITUTE(A246," ","_"),"_",B246)</f>
+        <v>Water_Sensor_water</v>
+      </c>
+      <c r="G246" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="247" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>155</v>
       </c>
@@ -6679,8 +7948,15 @@
       <c r="D247" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="248" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F247" t="str">
+        <f t="shared" si="60"/>
+        <v>Water_Sensor_water</v>
+      </c>
+      <c r="G247" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="248" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>157</v>
       </c>
@@ -6693,8 +7969,12 @@
       <c r="D248" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="249" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F248" t="str">
+        <f t="shared" si="60"/>
+        <v>Window_Shade_windowShade</v>
+      </c>
+    </row>
+    <row r="249" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>157</v>
       </c>
@@ -6707,8 +7987,12 @@
       <c r="D249" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="250" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F249" t="str">
+        <f t="shared" si="60"/>
+        <v>Window_Shade_windowShade</v>
+      </c>
+    </row>
+    <row r="250" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>157</v>
       </c>
@@ -6721,8 +8005,12 @@
       <c r="D250" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="251" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F250" t="str">
+        <f t="shared" si="60"/>
+        <v>Window_Shade_windowShade</v>
+      </c>
+    </row>
+    <row r="251" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>157</v>
       </c>
@@ -6735,8 +8023,12 @@
       <c r="D251" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="252" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F251" t="str">
+        <f t="shared" si="60"/>
+        <v>Window_Shade_windowShade</v>
+      </c>
+    </row>
+    <row r="252" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>157</v>
       </c>
@@ -6749,8 +8041,12 @@
       <c r="D252" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="253" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F252" t="str">
+        <f t="shared" si="60"/>
+        <v>Window_Shade_windowShade</v>
+      </c>
+    </row>
+    <row r="253" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>157</v>
       </c>
@@ -6763,8 +8059,12 @@
       <c r="D253" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F253" t="str">
+        <f t="shared" si="60"/>
+        <v>Window_Shade_windowShade</v>
+      </c>
+    </row>
+    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>157</v>
       </c>
@@ -6772,7 +8072,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="255" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>170</v>
       </c>
@@ -6782,8 +8082,12 @@
       <c r="C255" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="256" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F255" t="str">
+        <f t="shared" si="60"/>
+        <v>Zw_Multichannel_epEvent</v>
+      </c>
+    </row>
+    <row r="256" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>170</v>
       </c>
@@ -6792,6 +8096,10 @@
       </c>
       <c r="C256" t="s">
         <v>221</v>
+      </c>
+      <c r="F256" t="str">
+        <f t="shared" si="60"/>
+        <v>Zw_Multichannel_epInfo</v>
       </c>
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.25">
@@ -6827,14 +8135,14 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H260">
-    <filterColumn colId="2">
-      <filters blank="1"/>
-    </filterColumn>
+  <autoFilter ref="A1:K260">
     <filterColumn colId="4">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
       </customFilters>
+    </filterColumn>
+    <filterColumn colId="7">
+      <filters blank="1"/>
     </filterColumn>
   </autoFilter>
   <sortState ref="A1:E325">

</xml_diff>